<commit_message>
monje, paladín y pícaro XGE
</commit_message>
<xml_diff>
--- a/excels/Trad PHB.xlsx
+++ b/excels/Trad PHB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="326" yWindow="95" windowWidth="25349" windowHeight="11167" tabRatio="854" activeTab="10"/>
+    <workbookView xWindow="326" yWindow="95" windowWidth="25349" windowHeight="11167" tabRatio="854" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Indice" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3015" uniqueCount="2612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3015" uniqueCount="2613">
   <si>
     <t>Introducción</t>
   </si>
@@ -7882,6 +7882,9 @@
   </si>
   <si>
     <t>radiante</t>
+  </si>
+  <si>
+    <t>Paladín</t>
   </si>
 </sst>
 </file>
@@ -9764,8 +9767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D362"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView topLeftCell="A329" workbookViewId="0">
+      <selection activeCell="B347" sqref="B347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -12689,8 +12692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AV12"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AG7" sqref="AG7"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -12777,7 +12780,7 @@
       </c>
       <c r="X2"/>
       <c r="Z2" s="10" t="s">
-        <v>2078</v>
+        <v>2612</v>
       </c>
       <c r="AA2" s="10" t="s">
         <v>2078</v>
@@ -17990,8 +17993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D197"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -19644,8 +19647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>